<commit_message>
juste avant de passer au template
</commit_message>
<xml_diff>
--- a/head_shot/Road_to_Ecolab.xlsx
+++ b/head_shot/Road_to_Ecolab.xlsx
@@ -646,7 +646,11 @@
           <t>EVENT Chromato</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr"/>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Vide_1</t>
+        </is>
+      </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>CONFIG_MES_INCUB</t>
@@ -752,7 +756,11 @@
           <t>EV_VIDANGE_CLIM</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr"/>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Vide_2</t>
+        </is>
+      </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>MAX T</t>
@@ -814,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>MOD(INT(C2/60),60)</f>
+        <f>MOD(INT(C2 /60),60)</f>
         <v/>
       </c>
       <c r="C2" t="n">
@@ -834,14 +842,17 @@
       <c r="G2" t="n">
         <v>0</v>
       </c>
-      <c r="H2" t="n">
-        <v>22</v>
-      </c>
-      <c r="I2" t="n">
-        <v>22</v>
-      </c>
-      <c r="J2" t="n">
-        <v>22</v>
+      <c r="H2">
+        <f>$F2</f>
+        <v/>
+      </c>
+      <c r="I2">
+        <f>$F2</f>
+        <v/>
+      </c>
+      <c r="J2">
+        <f>$F2</f>
+        <v/>
       </c>
       <c r="K2" t="n">
         <v>1</v>
@@ -1002,7 +1013,7 @@
         <v/>
       </c>
       <c r="B3">
-        <f>MOD(INT(C3/60),60)</f>
+        <f>MOD(INT(C3 /60),60)</f>
         <v/>
       </c>
       <c r="C3">
@@ -1023,14 +1034,17 @@
       <c r="G3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="n">
-        <v>22</v>
-      </c>
-      <c r="I3" t="n">
-        <v>22</v>
-      </c>
-      <c r="J3" t="n">
-        <v>22</v>
+      <c r="H3">
+        <f>$F3</f>
+        <v/>
+      </c>
+      <c r="I3">
+        <f>$F3</f>
+        <v/>
+      </c>
+      <c r="J3">
+        <f>$F3</f>
+        <v/>
       </c>
       <c r="K3" t="n">
         <v>1</v>
@@ -1191,7 +1205,7 @@
         <v/>
       </c>
       <c r="B4">
-        <f>MOD(INT(C4/60),60)</f>
+        <f>MOD(INT(C4 /60),60)</f>
         <v/>
       </c>
       <c r="C4">
@@ -1212,14 +1226,17 @@
       <c r="G4" t="n">
         <v>0</v>
       </c>
-      <c r="H4" t="n">
-        <v>22</v>
-      </c>
-      <c r="I4" t="n">
-        <v>22</v>
-      </c>
-      <c r="J4" t="n">
-        <v>22</v>
+      <c r="H4">
+        <f>$F4</f>
+        <v/>
+      </c>
+      <c r="I4">
+        <f>$F4</f>
+        <v/>
+      </c>
+      <c r="J4">
+        <f>$F4</f>
+        <v/>
       </c>
       <c r="K4" t="n">
         <v>1</v>
@@ -1380,7 +1397,7 @@
         <v/>
       </c>
       <c r="B5">
-        <f>MOD(INT(C5/60),60)</f>
+        <f>MOD(INT(C5 /60),60)</f>
         <v/>
       </c>
       <c r="C5">
@@ -1401,14 +1418,17 @@
       <c r="G5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="n">
-        <v>22</v>
-      </c>
-      <c r="I5" t="n">
-        <v>22</v>
-      </c>
-      <c r="J5" t="n">
-        <v>22</v>
+      <c r="H5">
+        <f>$F5</f>
+        <v/>
+      </c>
+      <c r="I5">
+        <f>$F5</f>
+        <v/>
+      </c>
+      <c r="J5">
+        <f>$F5</f>
+        <v/>
       </c>
       <c r="K5" t="n">
         <v>1</v>
@@ -1569,7 +1589,7 @@
         <v/>
       </c>
       <c r="B6">
-        <f>MOD(INT(C6/60),60)</f>
+        <f>MOD(INT(C6 /60),60)</f>
         <v/>
       </c>
       <c r="C6">
@@ -1590,14 +1610,17 @@
       <c r="G6" t="n">
         <v>0</v>
       </c>
-      <c r="H6" t="n">
-        <v>22</v>
-      </c>
-      <c r="I6" t="n">
-        <v>22</v>
-      </c>
-      <c r="J6" t="n">
-        <v>22</v>
+      <c r="H6">
+        <f>$F6</f>
+        <v/>
+      </c>
+      <c r="I6">
+        <f>$F6</f>
+        <v/>
+      </c>
+      <c r="J6">
+        <f>$F6</f>
+        <v/>
       </c>
       <c r="K6" t="n">
         <v>1</v>
@@ -1758,7 +1781,7 @@
         <v/>
       </c>
       <c r="B7">
-        <f>MOD(INT(C7/60),60)</f>
+        <f>MOD(INT(C7 /60),60)</f>
         <v/>
       </c>
       <c r="C7">
@@ -1779,14 +1802,17 @@
       <c r="G7" t="n">
         <v>0</v>
       </c>
-      <c r="H7" t="n">
-        <v>22</v>
-      </c>
-      <c r="I7" t="n">
-        <v>22</v>
-      </c>
-      <c r="J7" t="n">
-        <v>22</v>
+      <c r="H7">
+        <f>$F7</f>
+        <v/>
+      </c>
+      <c r="I7">
+        <f>$F7</f>
+        <v/>
+      </c>
+      <c r="J7">
+        <f>$F7</f>
+        <v/>
       </c>
       <c r="K7" t="n">
         <v>1</v>
@@ -1947,7 +1973,7 @@
         <v/>
       </c>
       <c r="B8">
-        <f>MOD(INT(C8/60),60)</f>
+        <f>MOD(INT(C8 /60),60)</f>
         <v/>
       </c>
       <c r="C8">
@@ -1968,14 +1994,17 @@
       <c r="G8" t="n">
         <v>0</v>
       </c>
-      <c r="H8" t="n">
-        <v>22</v>
-      </c>
-      <c r="I8" t="n">
-        <v>22</v>
-      </c>
-      <c r="J8" t="n">
-        <v>22</v>
+      <c r="H8">
+        <f>$F8</f>
+        <v/>
+      </c>
+      <c r="I8">
+        <f>$F8</f>
+        <v/>
+      </c>
+      <c r="J8">
+        <f>$F8</f>
+        <v/>
       </c>
       <c r="K8" t="n">
         <v>1</v>
@@ -2136,7 +2165,7 @@
         <v/>
       </c>
       <c r="B9">
-        <f>MOD(INT(C9/60),60)</f>
+        <f>MOD(INT(C9 /60),60)</f>
         <v/>
       </c>
       <c r="C9">
@@ -2157,14 +2186,17 @@
       <c r="G9" t="n">
         <v>0</v>
       </c>
-      <c r="H9" t="n">
-        <v>22</v>
-      </c>
-      <c r="I9" t="n">
-        <v>22</v>
-      </c>
-      <c r="J9" t="n">
-        <v>22</v>
+      <c r="H9">
+        <f>$F9</f>
+        <v/>
+      </c>
+      <c r="I9">
+        <f>$F9</f>
+        <v/>
+      </c>
+      <c r="J9">
+        <f>$F9</f>
+        <v/>
       </c>
       <c r="K9" t="n">
         <v>1</v>
@@ -2325,7 +2357,7 @@
         <v/>
       </c>
       <c r="B10">
-        <f>MOD(INT(C10/60),60)</f>
+        <f>MOD(INT(C10 /60),60)</f>
         <v/>
       </c>
       <c r="C10">
@@ -2346,14 +2378,17 @@
       <c r="G10" t="n">
         <v>0</v>
       </c>
-      <c r="H10" t="n">
-        <v>22</v>
-      </c>
-      <c r="I10" t="n">
-        <v>22</v>
-      </c>
-      <c r="J10" t="n">
-        <v>22</v>
+      <c r="H10">
+        <f>$F10</f>
+        <v/>
+      </c>
+      <c r="I10">
+        <f>$F10</f>
+        <v/>
+      </c>
+      <c r="J10">
+        <f>$F10</f>
+        <v/>
       </c>
       <c r="K10" t="n">
         <v>1</v>
@@ -2514,7 +2549,7 @@
         <v/>
       </c>
       <c r="B11">
-        <f>MOD(INT(C11/60),60)</f>
+        <f>MOD(INT(C11 /60),60)</f>
         <v/>
       </c>
       <c r="C11">
@@ -2535,14 +2570,17 @@
       <c r="G11" t="n">
         <v>0</v>
       </c>
-      <c r="H11" t="n">
-        <v>22</v>
-      </c>
-      <c r="I11" t="n">
-        <v>22</v>
-      </c>
-      <c r="J11" t="n">
-        <v>22</v>
+      <c r="H11">
+        <f>$F11</f>
+        <v/>
+      </c>
+      <c r="I11">
+        <f>$F11</f>
+        <v/>
+      </c>
+      <c r="J11">
+        <f>$F11</f>
+        <v/>
       </c>
       <c r="K11" t="n">
         <v>1</v>

</xml_diff>